<commit_message>
+ column detail san_pham
</commit_message>
<xml_diff>
--- a/file/E32 - Shop.xlsx
+++ b/file/E32 - Shop.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vieta\OneDrive\Desktop\tai_nguyen\new\Project_Shop\file\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\laragon\www\j2teamnnl\Project_Shop\file\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{327EF581-B5F6-49AD-98EF-EA477390307B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="612" windowWidth="23256" windowHeight="12456" activeTab="3"/>
+    <workbookView xWindow="-108" yWindow="612" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Khách hàng" sheetId="1" r:id="rId1"/>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="81">
   <si>
     <t>KHÁCH HÀNG</t>
   </si>
@@ -277,11 +278,14 @@
     <t>105 Hàng Bông, St, Hoàn
  Kiếm, Hà Nội, Việt Nam</t>
   </si>
+  <si>
+    <t>detail</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -490,7 +494,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -550,26 +554,8 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -592,6 +578,19 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -808,7 +807,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
@@ -31851,13 +31850,15 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:AB1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -32130,12 +32131,12 @@
       <c r="AB8" s="7"/>
     </row>
     <row r="9" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A9" s="27"/>
-      <c r="B9" s="28"/>
-      <c r="C9" s="28"/>
-      <c r="D9" s="28"/>
-      <c r="E9" s="28"/>
-      <c r="F9" s="28"/>
+      <c r="A9" s="32"/>
+      <c r="B9" s="33"/>
+      <c r="C9" s="33"/>
+      <c r="D9" s="33"/>
+      <c r="E9" s="33"/>
+      <c r="F9" s="33"/>
       <c r="G9" s="7"/>
       <c r="H9" s="7"/>
       <c r="I9" s="7"/>
@@ -61900,14 +61901,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:I10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -61923,18 +61924,18 @@
     <col min="9" max="9" width="21.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="27" t="s">
+    <row r="1" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A1" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
-      <c r="G1" s="28"/>
-      <c r="H1" s="28"/>
-      <c r="I1" s="28"/>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
+      <c r="I1" s="33"/>
     </row>
     <row r="2" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -61949,157 +61950,162 @@
       <c r="D2" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="F2" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="G2" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="G2" s="26" t="s">
+      <c r="H2" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="H2" s="23"/>
       <c r="I2" s="5"/>
     </row>
     <row r="3" spans="1:9" ht="37.799999999999997" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="33"/>
-      <c r="B3" s="33"/>
-      <c r="C3" s="34" t="s">
+      <c r="A3" s="25"/>
+      <c r="B3" s="25"/>
+      <c r="C3" s="26" t="s">
         <v>33</v>
       </c>
-      <c r="D3" s="34" t="s">
+      <c r="D3" s="26" t="s">
         <v>36</v>
       </c>
-      <c r="E3" s="33" t="s">
+      <c r="E3" s="26"/>
+      <c r="F3" s="25" t="s">
         <v>67</v>
       </c>
-      <c r="F3" s="35" t="s">
+      <c r="G3" s="27" t="s">
         <v>34</v>
       </c>
-      <c r="G3" s="33" t="s">
+      <c r="H3" s="25" t="s">
         <v>35</v>
       </c>
-      <c r="H3" s="24"/>
     </row>
     <row r="4" spans="1:9" ht="81.599999999999994" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="33"/>
-      <c r="B4" s="33"/>
-      <c r="C4" s="33" t="s">
+      <c r="A4" s="25"/>
+      <c r="B4" s="25"/>
+      <c r="C4" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="D4" s="34" t="s">
+      <c r="D4" s="26" t="s">
         <v>53</v>
       </c>
-      <c r="E4" s="33" t="s">
+      <c r="E4" s="26"/>
+      <c r="F4" s="25" t="s">
         <v>66</v>
       </c>
-      <c r="F4" s="33" t="s">
+      <c r="G4" s="25" t="s">
         <v>38</v>
       </c>
-      <c r="G4" s="33" t="s">
+      <c r="H4" s="25" t="s">
         <v>39</v>
       </c>
-      <c r="H4" s="24"/>
     </row>
     <row r="5" spans="1:9" ht="70.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="33"/>
-      <c r="B5" s="33"/>
-      <c r="C5" s="33" t="s">
+      <c r="A5" s="25"/>
+      <c r="B5" s="25"/>
+      <c r="C5" s="25" t="s">
         <v>47</v>
       </c>
-      <c r="D5" s="34" t="s">
+      <c r="D5" s="26" t="s">
         <v>54</v>
       </c>
-      <c r="E5" s="33" t="s">
+      <c r="E5" s="26"/>
+      <c r="F5" s="25" t="s">
         <v>65</v>
       </c>
-      <c r="F5" s="33" t="s">
+      <c r="G5" s="25" t="s">
         <v>44</v>
       </c>
-      <c r="G5" s="33" t="s">
+      <c r="H5" s="25" t="s">
         <v>40</v>
       </c>
-      <c r="H5" s="24"/>
     </row>
     <row r="6" spans="1:9" ht="37.799999999999997" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="33"/>
-      <c r="B6" s="33"/>
-      <c r="C6" s="33" t="s">
+      <c r="A6" s="25"/>
+      <c r="B6" s="25"/>
+      <c r="C6" s="25" t="s">
         <v>55</v>
       </c>
-      <c r="D6" s="34" t="s">
+      <c r="D6" s="26" t="s">
         <v>58</v>
       </c>
-      <c r="E6" s="33" t="s">
+      <c r="E6" s="26"/>
+      <c r="F6" s="25" t="s">
         <v>64</v>
       </c>
-      <c r="F6" s="33" t="s">
+      <c r="G6" s="25" t="s">
         <v>45</v>
       </c>
-      <c r="G6" s="33" t="s">
+      <c r="H6" s="25" t="s">
         <v>41</v>
       </c>
-      <c r="H6" s="25"/>
     </row>
     <row r="7" spans="1:9" ht="67.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="33"/>
-      <c r="B7" s="33"/>
-      <c r="C7" s="33" t="s">
+      <c r="A7" s="25"/>
+      <c r="B7" s="25"/>
+      <c r="C7" s="25" t="s">
         <v>48</v>
       </c>
-      <c r="D7" s="34" t="s">
+      <c r="D7" s="26" t="s">
         <v>56</v>
       </c>
-      <c r="E7" s="33" t="s">
+      <c r="E7" s="26"/>
+      <c r="F7" s="25" t="s">
         <v>63</v>
       </c>
-      <c r="F7" s="33" t="s">
+      <c r="G7" s="25" t="s">
         <v>57</v>
       </c>
-      <c r="G7" s="33" t="s">
+      <c r="H7" s="25" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="66.599999999999994" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="33"/>
-      <c r="B8" s="33"/>
-      <c r="C8" s="33" t="s">
+      <c r="A8" s="25"/>
+      <c r="B8" s="25"/>
+      <c r="C8" s="25" t="s">
         <v>49</v>
       </c>
-      <c r="D8" s="34" t="s">
+      <c r="D8" s="26" t="s">
         <v>59</v>
       </c>
-      <c r="E8" s="33" t="s">
+      <c r="E8" s="26"/>
+      <c r="F8" s="25" t="s">
         <v>62</v>
       </c>
-      <c r="F8" s="33" t="s">
+      <c r="G8" s="25" t="s">
         <v>46</v>
       </c>
-      <c r="G8" s="33" t="s">
+      <c r="H8" s="25" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="48" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="33"/>
-      <c r="B9" s="33"/>
-      <c r="C9" s="33" t="s">
+      <c r="A9" s="25"/>
+      <c r="B9" s="25"/>
+      <c r="C9" s="25" t="s">
         <v>50</v>
       </c>
-      <c r="D9" s="34" t="s">
+      <c r="D9" s="26" t="s">
         <v>60</v>
       </c>
-      <c r="E9" s="33" t="s">
+      <c r="E9" s="26"/>
+      <c r="F9" s="25" t="s">
         <v>61</v>
       </c>
-      <c r="F9" s="36" t="s">
+      <c r="G9" s="28" t="s">
         <v>51</v>
       </c>
-      <c r="G9" s="36" t="s">
+      <c r="H9" s="28" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="32" t="s">
+      <c r="A10" s="24" t="s">
         <v>32</v>
       </c>
     </row>
@@ -62113,14 +62119,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -62132,72 +62138,72 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="32" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
     </row>
     <row r="2" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A2" s="37" t="s">
+      <c r="A2" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="37" t="s">
+      <c r="B2" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="37" t="s">
+      <c r="C2" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="37" t="s">
+      <c r="D2" s="29" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="54.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="37"/>
-      <c r="B3" s="37" t="s">
+      <c r="A3" s="29"/>
+      <c r="B3" s="29" t="s">
         <v>68</v>
       </c>
-      <c r="C3" s="39" t="s">
+      <c r="C3" s="31" t="s">
         <v>72</v>
       </c>
-      <c r="D3" s="38" t="s">
+      <c r="D3" s="30" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="29.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="37"/>
-      <c r="B4" s="37" t="s">
+      <c r="A4" s="29"/>
+      <c r="B4" s="29" t="s">
         <v>69</v>
       </c>
-      <c r="C4" s="39" t="s">
+      <c r="C4" s="31" t="s">
         <v>73</v>
       </c>
-      <c r="D4" s="38" t="s">
+      <c r="D4" s="30" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="37"/>
-      <c r="B5" s="37" t="s">
+      <c r="A5" s="29"/>
+      <c r="B5" s="29" t="s">
         <v>70</v>
       </c>
-      <c r="C5" s="39" t="s">
+      <c r="C5" s="31" t="s">
         <v>74</v>
       </c>
-      <c r="D5" s="38" t="s">
+      <c r="D5" s="30" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="37"/>
-      <c r="B6" s="37" t="s">
+      <c r="A6" s="29"/>
+      <c r="B6" s="29" t="s">
         <v>71</v>
       </c>
-      <c r="C6" s="39" t="s">
+      <c r="C6" s="31" t="s">
         <v>75</v>
       </c>
-      <c r="D6" s="38" t="s">
+      <c r="D6" s="30" t="s">
         <v>79</v>
       </c>
     </row>
@@ -62206,17 +62212,17 @@
     <mergeCell ref="A1:D1"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="C3" r:id="rId1" display="https://www.randomphonenumbers.com/us_phone_number/212206-xxxx"/>
-    <hyperlink ref="C4" r:id="rId2" display="https://www.randomphonenumbers.com/us_phone_number/212209-xxxx"/>
-    <hyperlink ref="C5" r:id="rId3" display="https://www.randomphonenumbers.com/us_phone_number/212213-xxxx"/>
-    <hyperlink ref="C6" r:id="rId4" display="https://www.randomphonenumbers.com/us_phone_number/212221-xxxx"/>
+    <hyperlink ref="C3" r:id="rId1" display="https://www.randomphonenumbers.com/us_phone_number/212206-xxxx" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
+    <hyperlink ref="C4" r:id="rId2" display="https://www.randomphonenumbers.com/us_phone_number/212209-xxxx" xr:uid="{00000000-0004-0000-0300-000001000000}"/>
+    <hyperlink ref="C5" r:id="rId3" display="https://www.randomphonenumbers.com/us_phone_number/212213-xxxx" xr:uid="{00000000-0004-0000-0300-000002000000}"/>
+    <hyperlink ref="C6" r:id="rId4" display="https://www.randomphonenumbers.com/us_phone_number/212221-xxxx" xr:uid="{00000000-0004-0000-0300-000003000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
@@ -62306,7 +62312,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
@@ -62326,14 +62332,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="32" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
       <c r="G1" s="5"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -62404,7 +62410,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -62417,12 +62423,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="34" t="s">
         <v>31</v>
       </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
-      <c r="D1" s="31"/>
+      <c r="B1" s="35"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="36"/>
     </row>
     <row r="2" spans="1:4" ht="16.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="21" t="s">

</xml_diff>